<commit_message>
systemstatus cannot be null
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA3F5D3-8EF3-5842-B0C5-649C90A95A5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D677D95F-8904-6A4E-AB65-C59AC1999DA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_violent_warnings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="66">
   <si>
     <t>table_name</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>VWM</t>
-  </si>
-  <si>
-    <t>conditional_lookup</t>
   </si>
   <si>
     <t>warning_violent_lookup</t>
@@ -228,9 +225,6 @@
   </si>
   <si>
     <t>No Debt</t>
-  </si>
-  <si>
-    <t>DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -586,9 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -764,16 +758,16 @@
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="7"/>
       <c r="O5" s="9"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -784,7 +778,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -800,16 +794,16 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="7"/>
       <c r="O6" s="9"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -820,10 +814,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
@@ -834,18 +828,18 @@
       <c r="I7" s="8"/>
       <c r="K7" s="7"/>
       <c r="L7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -856,10 +850,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -873,16 +867,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
-        <v>67</v>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
       <c r="P9" s="6"/>
     </row>
@@ -2311,7 +2305,7 @@
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2480,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="9" t="s">
@@ -2488,16 +2482,16 @@
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -2508,7 +2502,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -2517,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
@@ -2525,16 +2519,16 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -2545,33 +2539,33 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9"/>
       <c r="K7" s="7"/>
       <c r="L7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -2582,10 +2576,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -2599,16 +2593,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
-        <v>67</v>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14">
@@ -4048,16 +4042,16 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
@@ -4088,10 +4082,10 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
@@ -4122,10 +4116,10 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="19"/>
@@ -4152,14 +4146,14 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="19"/>
@@ -4190,10 +4184,10 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="19"/>
@@ -32091,7 +32085,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -32217,7 +32211,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>23</v>
@@ -32264,24 +32258,22 @@
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -32292,7 +32284,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -32305,24 +32297,22 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -32333,10 +32323,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
@@ -32346,24 +32336,22 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -32374,10 +32362,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -32391,13 +32379,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14">
@@ -33825,7 +33816,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -33994,28 +33985,26 @@
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -34026,7 +34015,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -34035,28 +34024,26 @@
         <v>0</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -34067,37 +34054,35 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -34108,10 +34093,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -34125,13 +34110,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14">
@@ -35559,7 +35547,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -35685,7 +35673,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>23</v>
@@ -35732,24 +35720,22 @@
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -35760,7 +35746,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -35773,24 +35759,22 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="M6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -35801,10 +35785,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
@@ -35814,24 +35798,22 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -35842,10 +35824,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -35859,13 +35841,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14">
@@ -37293,7 +37278,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -37419,7 +37404,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>23</v>
@@ -37466,24 +37451,22 @@
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="M5" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15">
@@ -37494,7 +37477,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>26</v>
@@ -37507,24 +37490,22 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15">
@@ -37535,10 +37516,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="5" t="b">
         <v>0</v>
@@ -37548,24 +37529,22 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15">
@@ -37576,10 +37555,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
@@ -37593,13 +37572,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14">
@@ -39025,7 +39007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -39099,13 +39081,13 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -39114,18 +39096,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -39134,7 +39116,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14">

</xml_diff>

<commit_message>
title case all instances of 'other'
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CB8F54-355A-0948-9B04-233BF6DFDF3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4C1625-ACEC-354E-9540-27D6A6787CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="460" windowWidth="48620" windowHeight="21940" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="93">
   <si>
     <t>table_name</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>SAAR Check</t>
-  </si>
-  <si>
-    <t>OTHER</t>
   </si>
   <si>
     <t>Debt chase</t>
@@ -857,148 +854,148 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="H3" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>79</v>
-      </c>
       <c r="H4" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="H5" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>17</v>
@@ -1007,30 +1004,30 @@
         <v>17</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1229,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1267,7 +1264,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1562,7 +1559,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1597,7 +1594,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2201,7 +2198,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2237,7 +2234,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2532,7 +2529,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2568,7 +2565,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2864,7 +2861,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2900,7 +2897,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3008,7 +3005,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J5:J6"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3196,7 +3193,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="8"/>
       <c r="M5" s="4" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -3232,7 +3229,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="8"/>
       <c r="M6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3265,7 +3262,7 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8"/>
@@ -3412,13 +3409,13 @@
     </row>
     <row r="2" spans="1:26" ht="15">
       <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -3428,18 +3425,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -3449,7 +3446,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IN-920 fix default value of assignee_id for deputy special warnings
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Warnings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4C1625-ACEC-354E-9540-27D6A6787CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FDF87E-0019-3B4A-9607-B81D9A3B9285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="48620" windowHeight="21940" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30040" yWindow="6760" windowWidth="27680" windowHeight="18820" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="9" r:id="rId1"/>
@@ -851,6 +851,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="17" t="s">
@@ -1042,7 +1045,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2010,7 +2013,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2339,9 +2342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5:J6"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2473,7 +2476,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>24</v>
@@ -3002,7 +3005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>

</xml_diff>